<commit_message>
remade larval survival figure
</commit_message>
<xml_diff>
--- a/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-08-02-Larvae-Counts.xlsx
+++ b/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-08-02-Larvae-Counts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-oa/data/2017-07-30-pacific-oyster-larvae/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaaminivenkataraman/Documents/project-oyster-oa/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -384,7 +384,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -397,7 +397,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2800"/>
               <a:t>Live Larvae per Treatment</a:t>
             </a:r>
           </a:p>
@@ -417,7 +417,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -901,16 +901,79 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-585563424"/>
-        <c:axId val="-585559056"/>
+        <c:axId val="-1801521808"/>
+        <c:axId val="-1777736624"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-585563424"/>
+        <c:axId val="-1801521808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.436240186301749"/>
+              <c:y val="0.93630303030303"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -933,7 +996,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -948,7 +1011,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-585559056"/>
+        <c:crossAx val="-1777736624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -957,7 +1020,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-585559056"/>
+        <c:axId val="-1777736624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300000.0"/>
@@ -978,12 +1041,80 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
+                  <a:t> of Live Larvae</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.00732064421669107"/>
+              <c:y val="0.29585015509425"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
             </a:solidFill>
@@ -995,7 +1126,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1010,7 +1141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-585563424"/>
+        <c:crossAx val="-1801521808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1038,7 +1169,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -26257,7 +26388,7 @@
         <v>0</v>
       </c>
       <c r="Z339">
-        <f t="shared" ref="Z338:Z345" si="214">SUM(Q338:Q339)</f>
+        <f t="shared" ref="Z339:Z345" si="214">SUM(Q338:Q339)</f>
         <v>813.33333333333337</v>
       </c>
     </row>

</xml_diff>

<commit_message>
consolidated larval counts into a new sheet
</commit_message>
<xml_diff>
--- a/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-08-02-Larvae-Counts.xlsx
+++ b/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-08-02-Larvae-Counts.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Chart1" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="53">
   <si>
     <t>Plate Number</t>
   </si>
@@ -251,8 +253,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -308,7 +312,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -330,6 +334,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -351,6 +356,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -901,11 +907,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1801521808"/>
-        <c:axId val="-1777736624"/>
+        <c:axId val="638206480"/>
+        <c:axId val="639956736"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-1801521808"/>
+        <c:axId val="638206480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,7 +1017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1777736624"/>
+        <c:crossAx val="639956736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1020,7 +1026,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-1777736624"/>
+        <c:axId val="639956736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300000.0"/>
@@ -1141,7 +1147,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1801521808"/>
+        <c:crossAx val="638206480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1764,7 +1770,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2064,9 +2070,9 @@
   <dimension ref="A1:AB363"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A341" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A348" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="V355" sqref="V355"/>
+      <selection pane="bottomLeft" activeCell="Q316" sqref="Q316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28004,7 +28010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -28364,4 +28372,1083 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6">
+        <v>42946</v>
+      </c>
+      <c r="C1" s="6">
+        <v>42948</v>
+      </c>
+      <c r="D1" s="6">
+        <v>42950</v>
+      </c>
+      <c r="E1" s="6">
+        <v>42952</v>
+      </c>
+      <c r="F1" s="6">
+        <v>42954</v>
+      </c>
+      <c r="G1" s="6">
+        <v>42956</v>
+      </c>
+      <c r="H1" s="6">
+        <v>42958</v>
+      </c>
+      <c r="I1" s="6">
+        <v>42960</v>
+      </c>
+      <c r="J1" s="6">
+        <v>42962</v>
+      </c>
+      <c r="K1" s="6">
+        <v>42964</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>60000</v>
+      </c>
+      <c r="C2">
+        <v>55555.555555555562</v>
+      </c>
+      <c r="D2">
+        <f>SUM(Sheet1!Q26:Q27)</f>
+        <v>58500</v>
+      </c>
+      <c r="E2">
+        <v>41600</v>
+      </c>
+      <c r="F2">
+        <v>34666.666666666664</v>
+      </c>
+      <c r="G2" s="7">
+        <f>SUM(Sheet1!Q124:Q125)</f>
+        <v>23306.666666666668</v>
+      </c>
+      <c r="H2">
+        <f>SUM(Sheet1!Q172:Q173)</f>
+        <v>8533.3333333333339</v>
+      </c>
+      <c r="I2">
+        <f>SUM(Sheet1!Q220:Q221)</f>
+        <v>9600</v>
+      </c>
+      <c r="J2">
+        <f>SUM(Sheet1!Q268:Q269)</f>
+        <v>7286.6666666666661</v>
+      </c>
+      <c r="K2">
+        <f>SUM(Sheet1!Q316:Q317)</f>
+        <v>1760</v>
+      </c>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>60000</v>
+      </c>
+      <c r="C3">
+        <v>36111.111111111117</v>
+      </c>
+      <c r="D3">
+        <f>SUM(Sheet1!Q28:Q29)</f>
+        <v>74666.666666666672</v>
+      </c>
+      <c r="E3">
+        <v>34666.666666666664</v>
+      </c>
+      <c r="F3">
+        <v>26400</v>
+      </c>
+      <c r="G3" s="7">
+        <f>SUM(Sheet1!Q126:Q127)</f>
+        <v>24000</v>
+      </c>
+      <c r="H3">
+        <f>SUM(Sheet1!Q174:Q175)</f>
+        <v>10733.333333333334</v>
+      </c>
+      <c r="I3">
+        <f>SUM(Sheet1!Q222:Q223)</f>
+        <v>5200</v>
+      </c>
+      <c r="J3">
+        <f>SUM(Sheet1!Q270:Q271)</f>
+        <v>3666.6666666666665</v>
+      </c>
+      <c r="K3">
+        <f>SUM(Sheet1!Q318:Q319)</f>
+        <v>1106.6666666666667</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>60000</v>
+      </c>
+      <c r="C4">
+        <v>57777.777777777774</v>
+      </c>
+      <c r="D4">
+        <f>SUM(Sheet1!Q30:Q31)</f>
+        <v>42200</v>
+      </c>
+      <c r="E4">
+        <v>46400</v>
+      </c>
+      <c r="F4">
+        <v>36400</v>
+      </c>
+      <c r="G4" s="7">
+        <f>SUM(Sheet1!Q128:Q129)</f>
+        <v>23586.666666666664</v>
+      </c>
+      <c r="H4">
+        <f>SUM(Sheet1!Q176:Q177)</f>
+        <v>13933.333333333332</v>
+      </c>
+      <c r="I4">
+        <f>SUM(Sheet1!Q224:Q225)</f>
+        <v>11666.666666666668</v>
+      </c>
+      <c r="J4">
+        <f>SUM(Sheet1!Q272:Q273)</f>
+        <v>5300</v>
+      </c>
+      <c r="K4">
+        <f>SUM(Sheet1!Q320:Q321)</f>
+        <v>2133.3333333333335</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>60000</v>
+      </c>
+      <c r="C5">
+        <v>44444.444444444445</v>
+      </c>
+      <c r="D5">
+        <f>SUM(Sheet1!Q32:Q33)</f>
+        <v>39600</v>
+      </c>
+      <c r="E5">
+        <v>36000</v>
+      </c>
+      <c r="F5">
+        <v>36266.666666666664</v>
+      </c>
+      <c r="G5" s="7">
+        <f>SUM(Sheet1!Q130:Q131)</f>
+        <v>32653.333333333332</v>
+      </c>
+      <c r="H5">
+        <f>SUM(Sheet1!Q178:Q179)</f>
+        <v>12800</v>
+      </c>
+      <c r="I5">
+        <f>SUM(Sheet1!Q226:Q227)</f>
+        <v>8666.6666666666661</v>
+      </c>
+      <c r="J5">
+        <f>SUM(Sheet1!Q274:Q275)</f>
+        <v>4333.333333333333</v>
+      </c>
+      <c r="K5">
+        <f>SUM(Sheet1!Q322:Q323)</f>
+        <v>1866.666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>60000</v>
+      </c>
+      <c r="C6">
+        <v>53333.333333333336</v>
+      </c>
+      <c r="D6">
+        <f>SUM(Sheet1!Q34:Q35)</f>
+        <v>44733.333333333328</v>
+      </c>
+      <c r="E6">
+        <v>43680</v>
+      </c>
+      <c r="F6">
+        <v>33600</v>
+      </c>
+      <c r="G6" s="7">
+        <f>SUM(Sheet1!Q132:Q133)</f>
+        <v>25399.999999999996</v>
+      </c>
+      <c r="H6">
+        <f>SUM(Sheet1!Q180:Q181)</f>
+        <v>20160</v>
+      </c>
+      <c r="I6">
+        <f>SUM(Sheet1!Q228:Q229)</f>
+        <v>18000</v>
+      </c>
+      <c r="J6">
+        <f>SUM(Sheet1!Q276:Q277)</f>
+        <v>5133.3333333333339</v>
+      </c>
+      <c r="K6">
+        <f>SUM(Sheet1!Q324:Q325)</f>
+        <v>2666.666666666667</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>60000</v>
+      </c>
+      <c r="C7">
+        <v>52777.777777777781</v>
+      </c>
+      <c r="D7">
+        <f>SUM(Sheet1!Q36:Q37)</f>
+        <v>32733.333333333336</v>
+      </c>
+      <c r="E7">
+        <v>35520</v>
+      </c>
+      <c r="F7">
+        <v>24800</v>
+      </c>
+      <c r="G7" s="7">
+        <f>SUM(Sheet1!Q134:Q135)</f>
+        <v>8533.3333333333339</v>
+      </c>
+      <c r="H7">
+        <f>SUM(Sheet1!Q182:Q183)</f>
+        <v>10080</v>
+      </c>
+      <c r="I7">
+        <f>SUM(Sheet1!Q230:Q231)</f>
+        <v>8099.9999999999991</v>
+      </c>
+      <c r="J7">
+        <f>SUM(Sheet1!Q278:Q279)</f>
+        <v>3466.6666666666665</v>
+      </c>
+      <c r="K7">
+        <f>SUM(Sheet1!Q326:Q327)</f>
+        <v>1333.3333333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>60000</v>
+      </c>
+      <c r="C8">
+        <v>42222.222222222226</v>
+      </c>
+      <c r="D8">
+        <f>SUM(Sheet1!Q38:Q39)</f>
+        <v>35360</v>
+      </c>
+      <c r="E8">
+        <v>30766.666666666672</v>
+      </c>
+      <c r="F8">
+        <v>27200.000000000004</v>
+      </c>
+      <c r="G8" s="7">
+        <f>SUM(Sheet1!Q136:Q137)</f>
+        <v>25326.666666666664</v>
+      </c>
+      <c r="H8">
+        <f>SUM(Sheet1!Q184:Q185)</f>
+        <v>22200</v>
+      </c>
+      <c r="I8">
+        <f>SUM(Sheet1!Q232:Q233)</f>
+        <v>6000</v>
+      </c>
+      <c r="J8">
+        <f>SUM(Sheet1!Q280:Q281)</f>
+        <v>4866.666666666667</v>
+      </c>
+      <c r="K8">
+        <f>SUM(Sheet1!Q328:Q329)</f>
+        <v>1333.3333333333335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>60000</v>
+      </c>
+      <c r="C9">
+        <v>61333.333333333336</v>
+      </c>
+      <c r="D9">
+        <f>SUM(Sheet1!Q40:Q41)</f>
+        <v>37333.333333333336</v>
+      </c>
+      <c r="E9">
+        <v>32000</v>
+      </c>
+      <c r="F9">
+        <v>36833.333333333328</v>
+      </c>
+      <c r="G9" s="7">
+        <f>SUM(Sheet1!Q138:Q139)</f>
+        <v>38500</v>
+      </c>
+      <c r="H9">
+        <f>SUM(Sheet1!Q186:Q187)</f>
+        <v>14399.999999999998</v>
+      </c>
+      <c r="I9">
+        <f>SUM(Sheet1!Q234:Q235)</f>
+        <v>10633.333333333332</v>
+      </c>
+      <c r="J9">
+        <f>SUM(Sheet1!Q282:Q283)</f>
+        <v>5600</v>
+      </c>
+      <c r="K9">
+        <f>SUM(Sheet1!Q330:Q331)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>60000</v>
+      </c>
+      <c r="C10">
+        <v>75000</v>
+      </c>
+      <c r="D10">
+        <f>SUM(Sheet1!Q42:Q43)</f>
+        <v>44333.333333333336</v>
+      </c>
+      <c r="E10">
+        <v>48000</v>
+      </c>
+      <c r="F10">
+        <v>28999.999999999996</v>
+      </c>
+      <c r="G10" s="7">
+        <f>SUM(Sheet1!Q140:Q141)</f>
+        <v>32186.666666666668</v>
+      </c>
+      <c r="H10">
+        <f>SUM(Sheet1!Q188:Q189)</f>
+        <v>16791.666666666668</v>
+      </c>
+      <c r="I10">
+        <f>SUM(Sheet1!Q236:Q237)</f>
+        <v>9600</v>
+      </c>
+      <c r="J10">
+        <f>SUM(Sheet1!Q284:Q285)</f>
+        <v>6626.666666666667</v>
+      </c>
+      <c r="K10">
+        <f>SUM(Sheet1!Q332:Q333)</f>
+        <v>2840</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>60000</v>
+      </c>
+      <c r="C11">
+        <v>53333.333333333336</v>
+      </c>
+      <c r="D11">
+        <f>SUM(Sheet1!Q44:Q45)</f>
+        <v>39200</v>
+      </c>
+      <c r="E11">
+        <v>66750</v>
+      </c>
+      <c r="F11" s="3">
+        <v>42133.333333333336</v>
+      </c>
+      <c r="G11" s="7">
+        <f>SUM(Sheet1!Q142:Q143)</f>
+        <v>24026.666666666668</v>
+      </c>
+      <c r="H11">
+        <f>SUM(Sheet1!Q190:Q191)</f>
+        <v>13500</v>
+      </c>
+      <c r="I11">
+        <f>SUM(Sheet1!Q238:Q239)</f>
+        <v>12133.333333333334</v>
+      </c>
+      <c r="J11">
+        <f>SUM(Sheet1!Q286:Q287)</f>
+        <v>8600</v>
+      </c>
+      <c r="K11">
+        <f>SUM(Sheet1!Q334:Q335)</f>
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>60000</v>
+      </c>
+      <c r="C12">
+        <v>27777.777777777781</v>
+      </c>
+      <c r="D12">
+        <f>SUM(Sheet1!Q46:Q47)</f>
+        <v>44586.666666666664</v>
+      </c>
+      <c r="E12" s="3">
+        <v>46200</v>
+      </c>
+      <c r="F12">
+        <f>SUM(Sheet1!Q109,Sheet1!Q110)</f>
+        <v>32200</v>
+      </c>
+      <c r="G12" s="7">
+        <f>SUM(Sheet1!Q144:Q145)</f>
+        <v>22400</v>
+      </c>
+      <c r="H12">
+        <f>SUM(Sheet1!Q192:Q193)</f>
+        <v>15533.333333333334</v>
+      </c>
+      <c r="I12">
+        <f>SUM(Sheet1!Q240:Q241)</f>
+        <v>2333.3333333333335</v>
+      </c>
+      <c r="J12">
+        <f>SUM(Sheet1!Q288:Q289)</f>
+        <v>1466.6666666666665</v>
+      </c>
+      <c r="K12">
+        <f>SUM(Sheet1!Q336:Q337)</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>60000</v>
+      </c>
+      <c r="C13">
+        <v>47777.777777777781</v>
+      </c>
+      <c r="D13">
+        <f>SUM(Sheet1!Q48:Q49)</f>
+        <v>39900</v>
+      </c>
+      <c r="E13" s="3">
+        <v>41066.666666666672</v>
+      </c>
+      <c r="F13">
+        <v>23199.999999999996</v>
+      </c>
+      <c r="G13" s="7">
+        <f>SUM(Sheet1!Q146:Q147)</f>
+        <v>18973.333333333336</v>
+      </c>
+      <c r="H13">
+        <f>SUM(Sheet1!Q194:Q195)</f>
+        <v>15200</v>
+      </c>
+      <c r="I13">
+        <f>SUM(Sheet1!Q242:Q243)</f>
+        <v>2666.6666666666665</v>
+      </c>
+      <c r="J13">
+        <f>SUM(Sheet1!Q290:Q291)</f>
+        <v>1600</v>
+      </c>
+      <c r="K13">
+        <f>SUM(Sheet1!Q338:Q339)</f>
+        <v>813.33333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>60000</v>
+      </c>
+      <c r="C14">
+        <v>35555.555555555555</v>
+      </c>
+      <c r="D14">
+        <f>SUM(Sheet1!Q50:Q51)</f>
+        <v>32866.666666666664</v>
+      </c>
+      <c r="E14">
+        <v>40533.333333333336</v>
+      </c>
+      <c r="F14">
+        <v>26133.333333333332</v>
+      </c>
+      <c r="G14" s="7">
+        <f>SUM(Sheet1!Q148:Q149)</f>
+        <v>20706.666666666668</v>
+      </c>
+      <c r="H14">
+        <f>SUM(Sheet1!Q196:Q197)</f>
+        <v>13720.000000000002</v>
+      </c>
+      <c r="I14">
+        <f>SUM(Sheet1!Q244:Q245)</f>
+        <v>12266.666666666666</v>
+      </c>
+      <c r="J14">
+        <f>SUM(Sheet1!Q292:Q293)</f>
+        <v>6333.3333333333339</v>
+      </c>
+      <c r="K14">
+        <f>SUM(Sheet1!Q340:Q341)</f>
+        <v>1033.3333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>60000</v>
+      </c>
+      <c r="C15">
+        <v>51666.666666666664</v>
+      </c>
+      <c r="D15">
+        <f>SUM(Sheet1!Q52:Q53)</f>
+        <v>38266.666666666664</v>
+      </c>
+      <c r="E15">
+        <v>39100</v>
+      </c>
+      <c r="F15">
+        <v>40600</v>
+      </c>
+      <c r="G15" s="7">
+        <f>SUM(Sheet1!Q150:Q151)</f>
+        <v>25066.666666666664</v>
+      </c>
+      <c r="H15">
+        <f>SUM(Sheet1!Q198:Q199)</f>
+        <v>16000</v>
+      </c>
+      <c r="I15">
+        <f>SUM(Sheet1!Q246:Q247)</f>
+        <v>15066.666666666666</v>
+      </c>
+      <c r="J15">
+        <f>SUM(Sheet1!Q294:Q295)</f>
+        <v>9766.6666666666661</v>
+      </c>
+      <c r="K15">
+        <f>SUM(Sheet1!Q342:Q343)</f>
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>60000</v>
+      </c>
+      <c r="C16">
+        <v>31111.111111111113</v>
+      </c>
+      <c r="D16">
+        <f>SUM(Sheet1!Q54:Q55)</f>
+        <v>70640</v>
+      </c>
+      <c r="E16">
+        <v>26666.666666666668</v>
+      </c>
+      <c r="F16">
+        <v>40346.666666666672</v>
+      </c>
+      <c r="G16" s="7">
+        <f>SUM(Sheet1!Q152:Q153)</f>
+        <v>29233.333333333328</v>
+      </c>
+      <c r="H16">
+        <f>SUM(Sheet1!Q200:Q201)</f>
+        <v>13866.666666666668</v>
+      </c>
+      <c r="I16">
+        <f>SUM(Sheet1!Q248:Q249)</f>
+        <v>11200</v>
+      </c>
+      <c r="J16">
+        <f>SUM(Sheet1!Q296:Q297)</f>
+        <v>11920</v>
+      </c>
+      <c r="K16">
+        <f>SUM(Sheet1!Q344:Q345)</f>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>60000</v>
+      </c>
+      <c r="C17">
+        <v>42222.222222222226</v>
+      </c>
+      <c r="D17">
+        <f>SUM(Sheet1!Q56:Q57)</f>
+        <v>32000</v>
+      </c>
+      <c r="E17">
+        <v>26666.666666666668</v>
+      </c>
+      <c r="F17">
+        <v>21000</v>
+      </c>
+      <c r="G17" s="7">
+        <f>SUM(Sheet1!Q154:Q155)</f>
+        <v>25500</v>
+      </c>
+      <c r="H17">
+        <f>SUM(Sheet1!Q202:Q203)</f>
+        <v>12133.333333333332</v>
+      </c>
+      <c r="I17">
+        <f>SUM(Sheet1!Q250:Q251)</f>
+        <v>8066.666666666667</v>
+      </c>
+      <c r="J17">
+        <f>SUM(Sheet1!Q298:Q299)</f>
+        <v>1900</v>
+      </c>
+      <c r="K17">
+        <f>SUM(Sheet1!Q346:Q347)</f>
+        <v>833.33333333333337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>60000</v>
+      </c>
+      <c r="C18">
+        <v>51666.666666666664</v>
+      </c>
+      <c r="D18">
+        <f>SUM(Sheet1!Q58:Q59)</f>
+        <v>37200</v>
+      </c>
+      <c r="E18">
+        <v>37440</v>
+      </c>
+      <c r="F18">
+        <v>29500.000000000004</v>
+      </c>
+      <c r="G18" s="7">
+        <f>SUM(Sheet1!Q156:Q157)</f>
+        <v>9300</v>
+      </c>
+      <c r="H18">
+        <f>SUM(Sheet1!Q204:Q205)</f>
+        <v>2666.666666666667</v>
+      </c>
+      <c r="I18">
+        <f>SUM(Sheet1!Q252:Q253)</f>
+        <v>1400</v>
+      </c>
+      <c r="J18">
+        <f>SUM(Sheet1!Q300:Q301)</f>
+        <v>1466.6666666666665</v>
+      </c>
+      <c r="K18">
+        <f>SUM(Sheet1!Q348:Q349)</f>
+        <v>1333.3333333333335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>60000</v>
+      </c>
+      <c r="C19">
+        <v>50555.555555555555</v>
+      </c>
+      <c r="D19">
+        <f>SUM(Sheet1!Q60:Q61)</f>
+        <v>29066.666666666664</v>
+      </c>
+      <c r="E19">
+        <v>27733.333333333332</v>
+      </c>
+      <c r="F19">
+        <v>27733.333333333332</v>
+      </c>
+      <c r="G19" s="7">
+        <f>SUM(Sheet1!Q158:Q159)</f>
+        <v>16033.333333333334</v>
+      </c>
+      <c r="H19">
+        <f>SUM(Sheet1!Q206:Q207)</f>
+        <v>16133.333333333334</v>
+      </c>
+      <c r="I19">
+        <f>SUM(Sheet1!Q254:Q255)</f>
+        <v>5000</v>
+      </c>
+      <c r="J19">
+        <f>SUM(Sheet1!Q302:Q303)</f>
+        <v>4966.666666666667</v>
+      </c>
+      <c r="K19">
+        <f>SUM(Sheet1!Q350:Q351)</f>
+        <v>533.33333333333337</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>60000</v>
+      </c>
+      <c r="C20">
+        <v>49444.444444444445</v>
+      </c>
+      <c r="D20">
+        <f>SUM(Sheet1!Q62:Q63)</f>
+        <v>35960</v>
+      </c>
+      <c r="E20">
+        <v>36666.666666666664</v>
+      </c>
+      <c r="F20">
+        <v>38566.666666666664</v>
+      </c>
+      <c r="G20" s="7">
+        <f>SUM(Sheet1!Q160:Q161)</f>
+        <v>20000</v>
+      </c>
+      <c r="H20">
+        <f>SUM(Sheet1!Q208:Q209)</f>
+        <v>11200.000000000002</v>
+      </c>
+      <c r="I20">
+        <f>SUM(Sheet1!Q256:Q257)</f>
+        <v>10800</v>
+      </c>
+      <c r="J20">
+        <f>SUM(Sheet1!Q304:Q305)</f>
+        <v>6233.3333333333339</v>
+      </c>
+      <c r="K20">
+        <f>SUM(Sheet1!Q352:Q353)</f>
+        <v>266.66666666666669</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>60000</v>
+      </c>
+      <c r="C21">
+        <v>44444.444444444445</v>
+      </c>
+      <c r="D21">
+        <f>SUM(Sheet1!Q64:Q65)</f>
+        <v>35333.333333333336</v>
+      </c>
+      <c r="E21">
+        <v>31800</v>
+      </c>
+      <c r="F21">
+        <v>28000.000000000004</v>
+      </c>
+      <c r="G21" s="7">
+        <f>SUM(Sheet1!Q162:Q163)</f>
+        <v>23900</v>
+      </c>
+      <c r="H21">
+        <f>SUM(Sheet1!Q210:Q211)</f>
+        <v>8600</v>
+      </c>
+      <c r="I21">
+        <f>SUM(Sheet1!Q258:Q259)</f>
+        <v>7466.6666666666661</v>
+      </c>
+      <c r="J21">
+        <f>SUM(Sheet1!Q306:Q307)</f>
+        <v>5733.3333333333339</v>
+      </c>
+      <c r="K21">
+        <f>SUM(Sheet1!Q354:Q355)</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>60000</v>
+      </c>
+      <c r="C22">
+        <v>57222.222222222226</v>
+      </c>
+      <c r="D22">
+        <f>SUM(Sheet1!Q66:Q67)</f>
+        <v>23600</v>
+      </c>
+      <c r="E22">
+        <v>25226.666666666668</v>
+      </c>
+      <c r="F22">
+        <v>31666.666666666668</v>
+      </c>
+      <c r="G22" s="7">
+        <f>SUM(Sheet1!Q164:Q165)</f>
+        <v>17680</v>
+      </c>
+      <c r="H22">
+        <f>SUM(Sheet1!Q212:Q213)</f>
+        <v>10666.666666666668</v>
+      </c>
+      <c r="I22">
+        <f>SUM(Sheet1!Q260:Q261)</f>
+        <v>8800</v>
+      </c>
+      <c r="J22">
+        <f>SUM(Sheet1!Q308:Q309)</f>
+        <v>4700</v>
+      </c>
+      <c r="K22">
+        <f>SUM(Sheet1!Q356:Q357)</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>60000</v>
+      </c>
+      <c r="C23">
+        <v>40000</v>
+      </c>
+      <c r="D23">
+        <f>SUM(Sheet1!Q68:Q69)</f>
+        <v>35733.333333333336</v>
+      </c>
+      <c r="E23">
+        <v>36000</v>
+      </c>
+      <c r="F23">
+        <v>27653.333333333332</v>
+      </c>
+      <c r="G23" s="7">
+        <f>SUM(Sheet1!Q166:Q167)</f>
+        <v>20066.666666666668</v>
+      </c>
+      <c r="H23">
+        <f>SUM(Sheet1!Q214:Q215)</f>
+        <v>8500</v>
+      </c>
+      <c r="I23">
+        <f>SUM(Sheet1!Q262:Q263)</f>
+        <v>8000</v>
+      </c>
+      <c r="J23">
+        <f>SUM(Sheet1!Q310:Q311)</f>
+        <v>4906.666666666667</v>
+      </c>
+      <c r="K23">
+        <f>SUM(Sheet1!Q358:Q359)</f>
+        <v>1093.3333333333335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>60000</v>
+      </c>
+      <c r="C24">
+        <v>33333.333333333336</v>
+      </c>
+      <c r="D24">
+        <f>SUM(Sheet1!Q70:Q71)</f>
+        <v>18200</v>
+      </c>
+      <c r="E24">
+        <v>33000</v>
+      </c>
+      <c r="F24">
+        <v>19200</v>
+      </c>
+      <c r="G24" s="7">
+        <f>SUM(Sheet1!Q168:Q169)</f>
+        <v>20800</v>
+      </c>
+      <c r="H24">
+        <f>SUM(Sheet1!Q216:Q217)</f>
+        <v>10640</v>
+      </c>
+      <c r="I24">
+        <f>SUM(Sheet1!Q264:Q265)</f>
+        <v>5600</v>
+      </c>
+      <c r="J24">
+        <f>SUM(Sheet1!Q312:Q313)</f>
+        <v>5666.666666666667</v>
+      </c>
+      <c r="K24">
+        <f>SUM(Sheet1!Q360:Q361)</f>
+        <v>533.33333333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>60000</v>
+      </c>
+      <c r="C25">
+        <v>48333.333333333336</v>
+      </c>
+      <c r="D25">
+        <f>SUM(Sheet1!Q72:Q73)</f>
+        <v>44933.333333333336</v>
+      </c>
+      <c r="E25">
+        <v>36266.666666666664</v>
+      </c>
+      <c r="F25">
+        <v>24000</v>
+      </c>
+      <c r="G25" s="7">
+        <f>SUM(Sheet1!Q170:Q171)</f>
+        <v>20466.666666666668</v>
+      </c>
+      <c r="H25">
+        <f>SUM(Sheet1!Q218:Q219)</f>
+        <v>17600</v>
+      </c>
+      <c r="I25">
+        <f>SUM(Sheet1!Q266:Q267)</f>
+        <v>7000</v>
+      </c>
+      <c r="J25">
+        <f>SUM(Sheet1!Q314:Q315)</f>
+        <v>2333.3333333333335</v>
+      </c>
+      <c r="K25">
+        <f>SUM(Sheet1!Q362:Q363)</f>
+        <v>1333.3333333333335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="42" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M42" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A24" sqref="A1:A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>